<commit_message>
Final commit with Automatic Allure
</commit_message>
<xml_diff>
--- a/testData/NearbyDoctors_TestData.xlsx
+++ b/testData/NearbyDoctors_TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="17">
   <si>
     <t>Location</t>
   </si>
@@ -549,22 +549,22 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>